<commit_message>
First commit on branch dev
</commit_message>
<xml_diff>
--- a/Book1.xlsx
+++ b/Book1.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Bjoern\Developer\git-xltrail-workbooks\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{0E8C269B-AB74-4D61-9CD0-9A3AC9735C10}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{F87750DD-8927-4A50-BB5B-71DD370FF117}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="20040" windowHeight="5100" xr2:uid="{A2835CEA-F6F6-41AA-90F4-9843B3B9F7D3}"/>
   </bookViews>
@@ -27,7 +27,7 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1" uniqueCount="1">
   <si>
-    <t>master branch</t>
+    <t>dev</t>
   </si>
 </sst>
 </file>

</xml_diff>